<commit_message>
add external stats to 556 ammo sheet
</commit_message>
<xml_diff>
--- a/changes/556-ammo.xlsx
+++ b/changes/556-ammo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8835D54-425E-4AF7-B734-17DC5AE8F13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CD12CC-4D5E-4261-B5CE-112DB3315CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="556-ammo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>old</t>
   </si>
@@ -146,12 +159,21 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>vel loss</t>
+  </si>
+  <si>
+    <t>suppression</t>
+  </si>
+  <si>
+    <t>pen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -985,11 +1007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:AG7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,24 +1019,18 @@
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="L1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="V1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1058,61 +1074,28 @@
         <v>18</v>
       </c>
       <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U2" t="s">
-        <v>24</v>
-      </c>
       <c r="V2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="W2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -1138,60 +1121,30 @@
         <v>42</v>
       </c>
       <c r="O3">
-        <v>-2</v>
+        <f>AVERAGE(L3:N3)</f>
+        <v>47.333333333333336</v>
+      </c>
+      <c r="P3">
+        <v>40</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R3">
-        <v>0.1</v>
+        <v>0.91</v>
       </c>
       <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
+        <f>C3-D3*20-E3*0.8-F3-0.6-G3*5+I3/200+(O3-50)*1.5</f>
+        <v>-6.5999999999999961</v>
       </c>
       <c r="V3">
-        <v>0.04</v>
+        <v>3165</v>
       </c>
       <c r="W3">
-        <v>150</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>55</v>
-      </c>
-      <c r="AA3">
-        <v>50</v>
-      </c>
-      <c r="AB3">
-        <v>44</v>
-      </c>
-      <c r="AC3">
-        <f>AVERAGE(Z3:AB3)</f>
-        <v>49.666666666666664</v>
-      </c>
-      <c r="AD3">
-        <f>Q3-R3*20-S3*0.8-T3-0.6-U3*5+W3/200+(AC3-50)*1.5</f>
-        <v>-2.3500000000000036</v>
-      </c>
-      <c r="AF3">
-        <v>3165</v>
-      </c>
-      <c r="AG3">
         <v>1658.165</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -1226,60 +1179,30 @@
         <v>42</v>
       </c>
       <c r="O4">
-        <v>-2.8</v>
+        <f>AVERAGE(L4:N4)</f>
+        <v>47.333333333333336</v>
+      </c>
+      <c r="P4">
+        <v>40</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R4">
-        <v>0.09</v>
+        <v>0.8</v>
       </c>
       <c r="S4">
-        <v>-1</v>
-      </c>
-      <c r="T4">
-        <v>-2</v>
-      </c>
-      <c r="U4">
-        <v>0.1</v>
+        <f>C4-D4*20-E4*0.8-F4-0.6-G4*5+I4/200+(O4-50)*1.5</f>
+        <v>-7.7999999999999972</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="W4">
-        <v>175</v>
-      </c>
-      <c r="Y4">
-        <v>600</v>
-      </c>
-      <c r="Z4">
-        <v>53</v>
-      </c>
-      <c r="AA4">
-        <v>48</v>
-      </c>
-      <c r="AB4">
-        <v>42</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" ref="AC4:AC7" si="0">AVERAGE(Z4:AB4)</f>
-        <v>47.666666666666664</v>
-      </c>
-      <c r="AD4">
-        <f t="shared" ref="AD4:AD7" si="1">Q4-R4*20-S4*0.8-T4-0.6-U4*5+W4/200+(AC4-50)*1.5</f>
-        <v>-2.7250000000000032</v>
-      </c>
-      <c r="AF4">
-        <v>3200</v>
-      </c>
-      <c r="AG4">
         <v>1512</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -1314,60 +1237,30 @@
         <v>51</v>
       </c>
       <c r="O5">
-        <v>-4.8499999999999996</v>
+        <f>AVERAGE(L5:N5)</f>
+        <v>54.666666666666664</v>
+      </c>
+      <c r="P5">
+        <v>50</v>
       </c>
       <c r="Q5">
-        <v>-2</v>
+        <v>100</v>
       </c>
       <c r="R5">
-        <v>0.15</v>
+        <v>0.63</v>
       </c>
       <c r="S5">
-        <v>2</v>
-      </c>
-      <c r="T5">
-        <v>2</v>
-      </c>
-      <c r="U5">
-        <v>-0.05</v>
+        <f>C5-D5*20-E5*0.8-F5-0.6-G5*5+I5/200+(O5-50)*1.5</f>
+        <v>0.74999999999999645</v>
       </c>
       <c r="V5">
-        <v>-0.02</v>
+        <v>3060</v>
       </c>
       <c r="W5">
-        <v>100</v>
-      </c>
-      <c r="Y5">
-        <v>1000</v>
-      </c>
-      <c r="Z5">
-        <v>58</v>
-      </c>
-      <c r="AA5">
-        <v>55</v>
-      </c>
-      <c r="AB5">
-        <v>51</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="0"/>
-        <v>54.666666666666664</v>
-      </c>
-      <c r="AD5">
-        <f t="shared" si="1"/>
-        <v>-1.4500000000000028</v>
-      </c>
-      <c r="AF5">
-        <v>3060</v>
-      </c>
-      <c r="AG5">
         <v>1748</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -1402,60 +1295,30 @@
         <v>42</v>
       </c>
       <c r="O6">
-        <v>-6.3</v>
+        <f>AVERAGE(L6:N6)</f>
+        <v>47.333333333333336</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
       </c>
       <c r="Q6">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R6">
-        <v>0.14000000000000001</v>
+        <v>0.97</v>
       </c>
       <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>-0.2</v>
+        <f>C6-D6*20-E6*0.8-F6-0.6-G6*5+I6/200+(O6-50)*1.5</f>
+        <v>-12.099999999999996</v>
       </c>
       <c r="V6">
-        <v>0.1</v>
+        <v>2953</v>
       </c>
       <c r="W6">
-        <v>50</v>
-      </c>
-      <c r="Y6">
-        <v>2000</v>
-      </c>
-      <c r="Z6">
-        <v>58</v>
-      </c>
-      <c r="AA6">
-        <v>53</v>
-      </c>
-      <c r="AB6">
-        <v>46</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="0"/>
-        <v>52.333333333333336</v>
-      </c>
-      <c r="AD6">
-        <f t="shared" si="1"/>
-        <v>-1.4499999999999966</v>
-      </c>
-      <c r="AF6">
-        <v>2953</v>
-      </c>
-      <c r="AG6">
         <v>1620</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>40</v>
       </c>
@@ -1490,54 +1353,378 @@
         <v>38</v>
       </c>
       <c r="O7">
-        <v>-9.8000000000000007</v>
+        <f>AVERAGE(L7:N7)</f>
+        <v>50</v>
+      </c>
+      <c r="P7">
+        <v>80</v>
       </c>
       <c r="Q7">
+        <v>80</v>
+      </c>
+      <c r="R7">
+        <v>0.38</v>
+      </c>
+      <c r="S7">
+        <f>C7-D7*20-E7*0.8-F7-0.6-G7*5+I7/200+(O7-50)*1.5</f>
+        <v>-12</v>
+      </c>
+      <c r="V7">
+        <v>3340</v>
+      </c>
+      <c r="W7">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="R7">
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.04</v>
+      </c>
+      <c r="I10">
+        <v>150</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>55</v>
+      </c>
+      <c r="M10">
+        <v>50</v>
+      </c>
+      <c r="N10">
+        <v>44</v>
+      </c>
+      <c r="O10">
+        <f>AVERAGE(L10:N10)</f>
+        <v>49.666666666666664</v>
+      </c>
+      <c r="P10">
+        <v>40</v>
+      </c>
+      <c r="Q10">
+        <v>30</v>
+      </c>
+      <c r="R10">
+        <v>0.8</v>
+      </c>
+      <c r="S10">
+        <f>C10-D10*20-E10*0.8-F10-0.6-G10*5+I10/200+(O10-50)</f>
+        <v>-2.1833333333333358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.09</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>-2</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>175</v>
+      </c>
+      <c r="K11">
+        <v>600</v>
+      </c>
+      <c r="L11">
+        <v>53</v>
+      </c>
+      <c r="M11">
+        <v>48</v>
+      </c>
+      <c r="N11">
+        <v>42</v>
+      </c>
+      <c r="O11">
+        <f>AVERAGE(L11:N11)</f>
+        <v>47.666666666666664</v>
+      </c>
+      <c r="P11">
+        <v>40</v>
+      </c>
+      <c r="Q11">
+        <v>60</v>
+      </c>
+      <c r="R11">
+        <v>0.6</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ref="S11:S14" si="0">C11-D11*20-E11*0.8-F11-0.6-G11*5+I11/200+(O11-50)</f>
+        <v>-1.5583333333333353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>-2</v>
+      </c>
+      <c r="D12">
+        <v>0.15</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>-0.05</v>
+      </c>
+      <c r="H12">
+        <v>-0.02</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>58</v>
+      </c>
+      <c r="M12">
+        <v>55</v>
+      </c>
+      <c r="N12">
+        <v>51</v>
+      </c>
+      <c r="O12">
+        <f>AVERAGE(L12:N12)</f>
+        <v>54.666666666666664</v>
+      </c>
+      <c r="P12">
+        <v>30</v>
+      </c>
+      <c r="Q12">
+        <v>50</v>
+      </c>
+      <c r="R12">
+        <v>0.7</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>-3.783333333333335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>-0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.1</v>
+      </c>
+      <c r="I13">
+        <v>50</v>
+      </c>
+      <c r="K13">
+        <v>2000</v>
+      </c>
+      <c r="L13">
+        <v>58</v>
+      </c>
+      <c r="M13">
+        <v>53</v>
+      </c>
+      <c r="N13">
+        <v>46</v>
+      </c>
+      <c r="O13">
+        <f>AVERAGE(L13:N13)</f>
+        <v>52.333333333333336</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
+      <c r="Q13">
+        <v>50</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>-2.6166666666666645</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
         <v>0.08</v>
       </c>
-      <c r="S7">
+      <c r="E14">
         <v>3</v>
       </c>
-      <c r="T7">
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="U7">
+      <c r="G14">
         <v>0.3</v>
       </c>
-      <c r="V7">
+      <c r="H14">
         <v>0</v>
       </c>
-      <c r="W7">
+      <c r="I14">
         <v>200</v>
       </c>
-      <c r="Y7">
+      <c r="K14">
         <v>1200</v>
       </c>
-      <c r="Z7">
+      <c r="L14">
         <v>65</v>
       </c>
-      <c r="AA7">
+      <c r="M14">
         <v>53</v>
       </c>
-      <c r="AB7">
+      <c r="N14">
         <v>40</v>
       </c>
-      <c r="AC7">
+      <c r="O14">
+        <f>AVERAGE(L14:N14)</f>
+        <v>52.666666666666664</v>
+      </c>
+      <c r="P14">
+        <v>80</v>
+      </c>
+      <c r="Q14">
+        <v>40</v>
+      </c>
+      <c r="R14">
+        <v>0.3</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="0"/>
-        <v>52.666666666666664</v>
-      </c>
-      <c r="AD7">
-        <f t="shared" si="1"/>
-        <v>-2.1000000000000032</v>
-      </c>
-      <c r="AF7">
-        <v>3340</v>
-      </c>
-      <c r="AG7">
-        <v>1844</v>
+        <v>-3.4333333333333353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>